<commit_message>
Update the verified dashboard metrics for shop-insight-v2
</commit_message>
<xml_diff>
--- a/TestData/Report/finances_summary_report.xlsx
+++ b/TestData/Report/finances_summary_report.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Variable</t>
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>total_orders</t>
   </si>
   <si>
     <t>gross_sales</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,7 +105,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1707.31</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
@@ -110,7 +113,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-43.76</v>
+        <v>3414.62</v>
       </c>
     </row>
     <row r="4">
@@ -118,7 +121,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-237.65</v>
+        <v>-87.52</v>
       </c>
     </row>
     <row r="5">
@@ -126,7 +129,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>19.51</v>
+        <v>-475.3</v>
       </c>
     </row>
     <row r="6">
@@ -134,7 +137,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>36.13</v>
+        <v>39.02</v>
       </c>
     </row>
     <row r="7">
@@ -142,7 +145,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>97.44</v>
+        <v>72.26</v>
       </c>
     </row>
     <row r="8">
@@ -150,6 +153,14 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
+        <v>194.88</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>